<commit_message>
updated graphs for jq
</commit_message>
<xml_diff>
--- a/report/JiakBot v1.0 Eval.xlsx
+++ b/report/JiakBot v1.0 Eval.xlsx
@@ -9,16 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8904" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8904" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="JiakBot v1.0 Evaluation" sheetId="3" r:id="rId1"/>
     <sheet name="JiakBot v1.0 Results" sheetId="4" r:id="rId2"/>
-    <sheet name="JiakBot v1.0 Evaluation + Human" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId3"/>
+    <sheet name="JiakBot v1.0 Evaluation + Human" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'JiakBot v1.0 Evaluation'!$A$1:$K$58</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'JiakBot v1.0 Evaluation + Human'!$A$1:$K$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'JiakBot v1.0 Evaluation + Human'!$A$1:$K$87</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="185">
   <si>
     <t>Greeting</t>
   </si>
@@ -619,6 +620,30 @@
   </si>
   <si>
     <t>Types of user inputs (%)</t>
+  </si>
+  <si>
+    <t>Greeting v1</t>
+  </si>
+  <si>
+    <t>Greeting v2</t>
+  </si>
+  <si>
+    <t>Statement v1</t>
+  </si>
+  <si>
+    <t>Statement v2</t>
+  </si>
+  <si>
+    <t>Question v1</t>
+  </si>
+  <si>
+    <t>Question v2</t>
+  </si>
+  <si>
+    <t>Rhetorical v1</t>
+  </si>
+  <si>
+    <t>Rhetorical v2</t>
   </si>
 </sst>
 </file>
@@ -850,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -890,6 +915,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -926,6 +952,2221 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-SG"/>
+              <a:t>JiakBot v1.0 -&gt; JiakBot</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-SG" baseline="0"/>
+              <a:t> v2.0</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-SG"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Inappropriate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$10:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Greeting v1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Greeting v2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Statement v1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Statement v2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Question v1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Question v2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Rhetorical v1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Rhetorical v2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$B$10:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.083333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28.645833333333332</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.541666666666666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.333333333333332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.666666666666664</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-333E-4DD2-AB33-0156BA14E80D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Appropriate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$10:$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Greeting v1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Greeting v2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Statement v1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Statement v2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Question v1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Question v2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Rhetorical v1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Rhetorical v2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$C$10:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>87.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.916666666666657</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.354166666666657</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>86.458333333333343</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81.666666666666671</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83.333333333333343</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.333333333333343</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-333E-4DD2-AB33-0156BA14E80D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1362403071"/>
+        <c:axId val="1362406815"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1362403071"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1362406815"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1362406815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG"/>
+                  <a:t>PERCENTAGE</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1362403071"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-SG"/>
+              <a:t>Type of user inputs (%)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$29:$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Greeting</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Statement</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Question</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Rhetorical</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$B$29:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>15.09433962264151</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.377358490566039</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.867924528301888</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6603773584905666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D5EC-40F9-9420-7C921D2EE963}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="315"/>
+        <c:overlap val="-40"/>
+        <c:axId val="1060130767"/>
+        <c:axId val="588368399"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1060130767"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="588368399"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="588368399"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1060130767"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="213">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3616,8 +5857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G7" sqref="F1:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3629,19 +5870,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
-      <c r="F1" s="21" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
+      <c r="F1" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="G1" s="23"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -3650,14 +5891,14 @@
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="F2" s="15" t="s">
+      <c r="D2" s="17"/>
+      <c r="F2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="16"/>
+      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4">
@@ -3668,20 +5909,20 @@
         <f>SUMIF('JiakBot v1.0 Evaluation'!$C$6:$C$58,"Greeting",'JiakBot v1.0 Evaluation'!$N$6:$N$58)</f>
         <v>42</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="17">
         <f>SUM(B3:C3)</f>
         <v>48</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="26">
+      <c r="F3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="27">
         <f>(D3/$D$7)*100</f>
         <v>15.09433962264151</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4">
@@ -3692,20 +5933,20 @@
         <f>SUMIF('JiakBot v1.0 Evaluation'!$C$6:$C$58,"Statement",'JiakBot v1.0 Evaluation'!$N$6:$N$58)</f>
         <v>137</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="17">
         <f>SUM(B4:C4)</f>
         <v>192</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="26">
+      <c r="F4" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="27">
         <f t="shared" ref="G4:G7" si="0">(D4/$D$7)*100</f>
         <v>60.377358490566039</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4">
@@ -3716,20 +5957,20 @@
         <f>SUMIF('JiakBot v1.0 Evaluation'!$C$6:$C$58,"Question",'JiakBot v1.0 Evaluation'!$N$6:$N$58)</f>
         <v>49</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="17">
         <f>SUM(B5:C5)</f>
         <v>60</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="27">
         <f t="shared" si="0"/>
         <v>18.867924528301888</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="16" t="s">
         <v>102</v>
       </c>
       <c r="B6" s="4">
@@ -3740,20 +5981,20 @@
         <f>SUMIF('JiakBot v1.0 Evaluation'!$C$6:$C$58,"Rhetorical",'JiakBot v1.0 Evaluation'!$N$6:$N$58)</f>
         <v>15</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="17">
         <f>SUM(B6:C6)</f>
         <v>18</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="27">
         <f t="shared" si="0"/>
         <v>5.6603773584905666</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="4">
@@ -3764,47 +6005,47 @@
         <f>SUM(C3:C6)</f>
         <v>243</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="17">
         <f>SUM(D3:D6)</f>
         <v>318</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="25">
+      <c r="F7" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="26">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="28">
         <f>(B7/$D$7)*100</f>
         <v>23.584905660377359</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="28">
         <f>(C7/$D$7)*100</f>
         <v>76.415094339622641</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="19">
         <f>(D7/$D$7)*100</f>
         <v>100</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="24"/>
+      <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -3813,108 +6054,108 @@
       <c r="C10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="20">
+      <c r="A11" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="21">
         <f>B3/$D3*100</f>
         <v>12.5</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="21">
         <f>C3/$D$3*100</f>
         <v>87.5</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="17">
         <f>SUM(B11:C11)</f>
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="20">
+      <c r="A12" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="21">
         <f t="shared" ref="B12:C15" si="1">B4/$D4*100</f>
         <v>28.645833333333332</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="21">
         <f t="shared" si="1"/>
         <v>71.354166666666657</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="17">
         <f>SUM(B12:C12)</f>
         <v>99.999999999999986</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="21">
         <f t="shared" si="1"/>
         <v>18.333333333333332</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="21">
         <f t="shared" si="1"/>
         <v>81.666666666666671</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="17">
         <f>SUM(B13:C13)</f>
         <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="21">
         <f t="shared" si="1"/>
         <v>16.666666666666664</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="21">
         <f t="shared" si="1"/>
         <v>83.333333333333343</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="17">
         <f>SUM(B14:C14)</f>
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="20">
+      <c r="A15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="21">
         <f>SUM(B11:B14)</f>
         <v>76.145833333333314</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="21">
         <f>SUM(C11:C14)</f>
         <v>323.85416666666663</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="17">
         <f>SUM(D11:D14)</f>
         <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="28">
         <f>(B15/D15)*100</f>
         <v>19.036458333333329</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="28">
         <f>(C15/D15)*100</f>
         <v>80.963541666666657</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="19">
         <f>B16+C16</f>
         <v>99.999999999999986</v>
       </c>
@@ -3931,6 +6172,295 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>12.5</v>
+      </c>
+      <c r="C2">
+        <v>87.5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>2.083333333333333</v>
+      </c>
+      <c r="G2">
+        <v>97.916666666666657</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>28.645833333333332</v>
+      </c>
+      <c r="C3">
+        <v>71.354166666666657</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>13.541666666666666</v>
+      </c>
+      <c r="G3">
+        <v>86.458333333333343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>18.333333333333332</v>
+      </c>
+      <c r="C4">
+        <v>81.666666666666671</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5">
+        <v>16.666666666666664</v>
+      </c>
+      <c r="C5">
+        <v>83.333333333333343</v>
+      </c>
+      <c r="E5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5">
+        <v>16.666666666666664</v>
+      </c>
+      <c r="G5">
+        <v>83.333333333333343</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>19.036458333333329</v>
+      </c>
+      <c r="C6">
+        <v>80.963541666666657</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>10.572916666666666</v>
+      </c>
+      <c r="G6">
+        <v>89.427083333333343</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10">
+        <v>12.5</v>
+      </c>
+      <c r="C10">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11">
+        <v>2.083333333333333</v>
+      </c>
+      <c r="C11">
+        <v>97.916666666666657</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B12">
+        <v>28.645833333333332</v>
+      </c>
+      <c r="C12">
+        <v>71.354166666666657</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13">
+        <v>13.541666666666666</v>
+      </c>
+      <c r="C13">
+        <v>86.458333333333343</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14">
+        <v>18.333333333333332</v>
+      </c>
+      <c r="C14">
+        <v>81.666666666666671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>183</v>
+      </c>
+      <c r="B16">
+        <v>16.666666666666664</v>
+      </c>
+      <c r="C16">
+        <v>83.333333333333343</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17">
+        <v>16.666666666666664</v>
+      </c>
+      <c r="C17">
+        <v>83.333333333333343</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="15">
+        <v>15.09433962264151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="15">
+        <v>60.377358490566039</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="15">
+        <v>18.867924528301888</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="15">
+        <v>5.6603773584905666</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R87"/>

</xml_diff>